<commit_message>
remove controller test from mt
</commit_message>
<xml_diff>
--- a/regulus/test/module_spec.xlsx
+++ b/regulus/test/module_spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -69,10 +69,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Confirmation_Controller#show</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Confirmation_Controller#update_graph</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -94,10 +90,6 @@
   </si>
   <si>
     <t>Information_Controller#get_tweet</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>URL(http://160.16.66.112:880)にアクセス</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -107,16 +99,6 @@
     </rPh>
     <rPh sb="5" eb="7">
       <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザにグラフとツイートと記事が表示されている</t>
-    <rPh sb="14" eb="16">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -791,7 +773,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -886,36 +868,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -1152,7 +1104,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1162,41 +1114,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1624,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F19"/>
+  <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1655,292 +1602,275 @@
       </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="5">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="10">
+        <v>3</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="10">
+        <v>4</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="10">
+        <v>6</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="10">
+        <v>7</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="10">
+        <v>9</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="10">
+        <v>10</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="10">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="C13" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="10">
+        <v>12</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="12">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="21" t="s">
+      <c r="F14" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="10">
+        <v>13</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="10">
         <v>14</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="12">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="22" t="s">
+      <c r="C16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="10">
         <v>15</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="12">
-        <v>4</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="12">
+      <c r="C17" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="12">
-        <v>6</v>
-      </c>
-      <c r="C8" s="18" t="s">
+      <c r="D17" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="19" thickBot="1">
+      <c r="B18" s="13">
+        <v>16</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="12">
-        <v>7</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="12">
-        <v>8</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="12">
-        <v>9</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="12">
-        <v>11</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="12">
-        <v>12</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="14" t="s">
+      <c r="D18" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="12">
-        <v>13</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="12">
-        <v>14</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="E18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="12">
-        <v>15</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="12">
-        <v>16</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="19" thickBot="1">
-      <c r="B19" s="15">
-        <v>17</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1959,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1994,133 +1924,133 @@
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="10">
+        <v>3</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="10">
+        <v>4</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="10">
+        <v>6</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F8" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="10">
+        <v>7</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="19" thickBot="1">
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="12">
-        <v>2</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="12">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="12">
-        <v>4</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="12">
-        <v>5</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="12">
-        <v>6</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="12">
-        <v>7</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="19" thickBot="1">
-      <c r="B10" s="15">
-        <v>8</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify mt spec for regulus
</commit_message>
<xml_diff>
--- a/regulus/test/module_spec.xlsx
+++ b/regulus/test/module_spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -57,497 +57,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>HTTP_Client#parse</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Confirmation_Controller#update_graph</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Information_Controller#get_article</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>HTTP_Client#parse</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Confirmation_Controller#update_graph</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Confirmation_Controller#update_view</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Currency_Controller#get_currncy</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>HTTP_Client#http_get</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>HTTP_Client#http_get</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Information_Controller#get_tweet</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>通貨情報を取得できている</t>
-    <rPh sb="0" eb="4">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メソッドを引数なしで実行</t>
-    <rPh sb="5" eb="7">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>外部サイトから通貨情報を含んだレスポンスを取得できている</t>
-    <rPh sb="0" eb="2">
-      <t>ガイブ</t>
-    </rPh>
-    <rPh sb="7" eb="11">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>レスポンスから通貨情報を抜き出している</t>
-    <rPh sb="7" eb="11">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ヌ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>ダ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>通貨情報を引数に指定してメソッドを実行</t>
-    <rPh sb="0" eb="4">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザに表示されているグラフが更新されている</t>
-    <rPh sb="5" eb="7">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メソッドを引数なしで実行</t>
-    <rPh sb="5" eb="7">
-      <t>ヒキスウナ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイートを取得できている</t>
-    <rPh sb="5" eb="7">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>日経の記事を取得できている</t>
-    <rPh sb="0" eb="2">
-      <t>ニッケイ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Confirmation_Controller#update_view</t>
-  </si>
-  <si>
-    <t>Confirmation_Controller#update_view</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Confirmation_Controller#update_view</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイートと記事を引数に指定してメソッドを実行（ツイート・記事がない場合）</t>
-    <rPh sb="5" eb="7">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイートと記事を引数に指定してメソッドを実行（ツイート・記事が両方ともある場合）</t>
-    <rPh sb="5" eb="7">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>リョウホウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイートと記事を引数に指定してメソッドを実行（ツイートのみがある場合）</t>
-    <rPh sb="5" eb="7">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>シテイス</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイートと記事を引数に指定してメソッドを実行（記事のみがある場合）</t>
-    <rPh sb="5" eb="7">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザに表示されているツイート・記事が更新されていない</t>
-    <rPh sb="5" eb="7">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザに表示されているツイート・記事が更新されている</t>
-    <rPh sb="5" eb="7">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザに表示されているツイートが更新されている</t>
-    <rPh sb="5" eb="7">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ブラウザに表示されている記事が更新されている</t>
-    <rPh sb="5" eb="7">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>通貨情報を含んだレスポンスを指定してメソッドを実行</t>
-    <rPh sb="0" eb="2">
-      <t>ツウカジョウホ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイートを含んだレスポンスを指定してメソッドを実行</t>
-    <rPh sb="5" eb="6">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>レスポンスからツイートを抜き出している</t>
-    <rPh sb="12" eb="13">
-      <t>ヌ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>ダ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>記事を含んだレスポンスを指定してメソッドを実行</t>
-    <rPh sb="0" eb="2">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>レスポンスから記事を抜き出している</t>
-    <rPh sb="7" eb="9">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ヌ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ダ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイートを含んだレスポンスを指定してメソッドを実行（ツイートが無かった場合）</t>
-    <rPh sb="5" eb="6">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>記事を含んだレスポンスを指定してメソッドを実行（記事が無かった場合）</t>
-    <rPh sb="0" eb="2">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>レスポンスから何も抜き出していない</t>
-    <rPh sb="7" eb="8">
-      <t>ナニ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ヌ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>ダ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>通貨情報取得のためのパスを指定してメソッドを実行</t>
-    <rPh sb="0" eb="4">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シュトク</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ツイート取得のためのパスを指定してメソッドを実行</t>
-    <rPh sb="4" eb="6">
-      <t>シュトク</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>記事取得のためのパスを指定してメソッドを実行</t>
-    <rPh sb="0" eb="4">
-      <t>キジシュトク</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ジッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>外部サイトからツイート情報を含んだレスポンスを取得できている</t>
-    <rPh sb="0" eb="2">
-      <t>ガイブ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>外部サイトから記事情報を含んだレスポンスを取得できている</t>
-    <rPh sb="0" eb="2">
-      <t>ガイブ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>キジ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ツウカジョウホウ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>シュトク</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -716,6 +238,71 @@
     </rPh>
     <rPh sb="11" eb="13">
       <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Currency::get_currencies</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正しく通貨情報を取得できている</t>
+    <rPh sb="0" eb="1">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>ツウカジョウホウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tweet::get_tweets</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pair, intervalを指定してメソッド実行</t>
+    <rPh sb="15" eb="17">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メソッド実行</t>
+    <rPh sb="4" eb="6">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正しくツイートを取得できている</t>
+    <rPh sb="0" eb="1">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Article::get_articles</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正しく記事を取得できている</t>
+    <rPh sb="0" eb="1">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>キジ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>シュトク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -773,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1006,6 +593,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1104,7 +749,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1140,12 +785,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="95">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -1571,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F18"/>
+  <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1609,13 +1257,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -1626,251 +1274,30 @@
         <v>4</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="10">
+    <row r="5" spans="2:6" ht="19" thickBot="1">
+      <c r="B5" s="21">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="10">
-        <v>4</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="10">
-        <v>5</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="10">
-        <v>6</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="10">
-        <v>7</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="10">
-        <v>8</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="10">
-        <v>9</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="10">
-        <v>10</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="10">
-        <v>11</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="10">
-        <v>12</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="10">
-        <v>13</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="D5" s="23" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="10">
-        <v>14</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="E5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="10">
-        <v>15</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="19" thickBot="1">
-      <c r="B18" s="13">
-        <v>16</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1925,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -1942,13 +1369,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:6">
@@ -1959,13 +1386,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:6">
@@ -1976,13 +1403,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -1993,13 +1420,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6">
@@ -2010,13 +1437,13 @@
         <v>5</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -2027,13 +1454,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="19" thickBot="1">
@@ -2044,13 +1471,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>